<commit_message>
Actualiacion de los archivos
</commit_message>
<xml_diff>
--- a/FusionFactory_Taxonomia_Productos_Artmode.xlsx
+++ b/FusionFactory_Taxonomia_Productos_Artmode.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\Archivos MAAJI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190F79B6-59A5-441D-9216-E8631A568802}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="8115" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -746,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>